<commit_message>
Remove UMC staff from selection
</commit_message>
<xml_diff>
--- a/collect_users/results/users_enriched.xlsx
+++ b/collect_users/results/users_enriched.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quach\OneDrive\Documents\GitHub\SWORDS-UU\collect_users\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beld\Documents\GitHub\SWORDS-UU\collect_users\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ACBA5D-E0EE-4651-B2BE-77AEF6CE3BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3A5DAF-8C84-4339-93FE-66B997A0488D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10477" uniqueCount="9181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10481" uniqueCount="9181">
   <si>
     <t>source</t>
   </si>
@@ -28129,8 +28129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2:AO491"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Z71" sqref="Z71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28463,10 +28463,10 @@
         <v>0</v>
       </c>
       <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>9147</v>
       </c>
       <c r="AN3" t="b">
         <v>0</v>
@@ -34279,7 +34279,7 @@
         <v>0</v>
       </c>
       <c r="AL58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM58" t="s">
         <v>9124</v>
@@ -35028,7 +35028,7 @@
         <v>0</v>
       </c>
       <c r="AL65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM65" t="s">
         <v>9146</v>
@@ -35245,7 +35245,7 @@
         <v>1</v>
       </c>
       <c r="AL67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM67">
         <v>0</v>
@@ -35358,7 +35358,7 @@
         <v>0</v>
       </c>
       <c r="AL68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM68">
         <v>0</v>
@@ -35584,7 +35584,7 @@
         <v>0</v>
       </c>
       <c r="AL70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM70" t="s">
         <v>9147</v>
@@ -37159,7 +37159,7 @@
         <v>0</v>
       </c>
       <c r="AL85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM85">
         <v>0</v>
@@ -52552,10 +52552,10 @@
         <v>0</v>
       </c>
       <c r="AL229">
-        <v>1</v>
-      </c>
-      <c r="AM229">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AM229" t="s">
+        <v>9147</v>
       </c>
       <c r="AN229" t="b">
         <v>0</v>
@@ -57070,7 +57070,7 @@
         <v>0</v>
       </c>
       <c r="AL271">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM271" t="s">
         <v>9147</v>
@@ -63115,7 +63115,7 @@
         <v>0</v>
       </c>
       <c r="AL328">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM328" t="s">
         <v>9165</v>
@@ -68634,7 +68634,10 @@
         <v>0</v>
       </c>
       <c r="AL380">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AM380" t="s">
+        <v>9147</v>
       </c>
       <c r="AN380" t="b">
         <v>1</v>
@@ -72889,7 +72892,7 @@
         <v>0</v>
       </c>
       <c r="AL421">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM421" t="s">
         <v>9138</v>
@@ -77980,7 +77983,10 @@
         <v>0</v>
       </c>
       <c r="AL469">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AM469" t="s">
+        <v>9147</v>
       </c>
       <c r="AN469" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Get readme and other repository data into all_variables file (#45)
</commit_message>
<xml_diff>
--- a/collect_users/results/users_enriched.xlsx
+++ b/collect_users/results/users_enriched.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quach\OneDrive\Documents\GitHub\SWORDS-UU\collect_users\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beld\Documents\GitHub\SWORDS-UU\collect_users\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ACBA5D-E0EE-4651-B2BE-77AEF6CE3BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3A5DAF-8C84-4339-93FE-66B997A0488D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10477" uniqueCount="9181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10481" uniqueCount="9181">
   <si>
     <t>source</t>
   </si>
@@ -28129,8 +28129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2:AO491"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Z71" sqref="Z71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28463,10 +28463,10 @@
         <v>0</v>
       </c>
       <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>9147</v>
       </c>
       <c r="AN3" t="b">
         <v>0</v>
@@ -34279,7 +34279,7 @@
         <v>0</v>
       </c>
       <c r="AL58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM58" t="s">
         <v>9124</v>
@@ -35028,7 +35028,7 @@
         <v>0</v>
       </c>
       <c r="AL65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM65" t="s">
         <v>9146</v>
@@ -35245,7 +35245,7 @@
         <v>1</v>
       </c>
       <c r="AL67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM67">
         <v>0</v>
@@ -35358,7 +35358,7 @@
         <v>0</v>
       </c>
       <c r="AL68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM68">
         <v>0</v>
@@ -35584,7 +35584,7 @@
         <v>0</v>
       </c>
       <c r="AL70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM70" t="s">
         <v>9147</v>
@@ -37159,7 +37159,7 @@
         <v>0</v>
       </c>
       <c r="AL85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM85">
         <v>0</v>
@@ -52552,10 +52552,10 @@
         <v>0</v>
       </c>
       <c r="AL229">
-        <v>1</v>
-      </c>
-      <c r="AM229">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AM229" t="s">
+        <v>9147</v>
       </c>
       <c r="AN229" t="b">
         <v>0</v>
@@ -57070,7 +57070,7 @@
         <v>0</v>
       </c>
       <c r="AL271">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM271" t="s">
         <v>9147</v>
@@ -63115,7 +63115,7 @@
         <v>0</v>
       </c>
       <c r="AL328">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM328" t="s">
         <v>9165</v>
@@ -68634,7 +68634,10 @@
         <v>0</v>
       </c>
       <c r="AL380">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AM380" t="s">
+        <v>9147</v>
       </c>
       <c r="AN380" t="b">
         <v>1</v>
@@ -72889,7 +72892,7 @@
         <v>0</v>
       </c>
       <c r="AL421">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM421" t="s">
         <v>9138</v>
@@ -77980,7 +77983,10 @@
         <v>0</v>
       </c>
       <c r="AL469">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AM469" t="s">
+        <v>9147</v>
       </c>
       <c r="AN469" t="b">
         <v>1</v>

</xml_diff>